<commit_message>
epochs Records & all properties
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -424,27 +424,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Epoch</t>
+          <t>epoch</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>loss</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>MAE</t>
+          <t>mae</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Val_Loss</t>
+          <t>val_loss</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Val_MAE</t>
+          <t>val_mae</t>
         </is>
       </c>
     </row>

</xml_diff>